<commit_message>
bug fix: hash_key should be required
</commit_message>
<xml_diff>
--- a/slalom/tests/resources/anon-test-anonymized.xlsx
+++ b/slalom/tests/resources/anon-test-anonymized.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,557 +439,491 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID Column</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>ID Column</t>
+          <t>Data Column A</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Data Column A</t>
+          <t>Data Column B</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Data Column B</t>
+          <t>Data Column C</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Data Column C</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
           <t>Data Column D</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>57893be3c23ca4276b1a6e6b1282ce81</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>747c6996c35bacb8b58008b74d048597</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>123</v>
+      <c r="C2" t="n">
+        <v>123</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>326720eccc03c79796a5967ef9498ce2</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>7a0d6760949ecfbddaa2d8f1ccf27368</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>123</v>
+      <c r="C3" t="n">
+        <v>123</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F3" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>e861ea0e5fa5454558cef99ea0d1f1f4</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>23cd35578cac237665f3a68882d5d66f</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
           <t>C</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>123</v>
+      <c r="C4" t="n">
+        <v>123</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F4" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>e97dd4b96679bf0a2dadcf1b236c0451</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>a63017b825525dae802c39c9a694797e</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>123</v>
+      <c r="C5" t="n">
+        <v>123</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F5" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>7010f4a26380f40f16c6951ded938bb1</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>588ed5aaaafefc734bd150ee89931468</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>123</v>
+      <c r="C6" t="n">
+        <v>123</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F6" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>f8ff17ebd49cbcd73d6b0230a60a8582</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>e9665c97c0e542ec92a06fd3971c6ffd</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
           <t>C</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>123</v>
+      <c r="C7" t="n">
+        <v>123</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F7" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>d97ef26a90e885fc56210aede0d357a5</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>161e235f3c3129884867791c9bd7f98e</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>123</v>
+      <c r="C8" t="n">
+        <v>123</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F8" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>b61c98e1519a53cb141f487a05d2b53c</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>baf5d3da11afdccadaccdf2722ede2f4</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>123</v>
+      <c r="C9" t="n">
+        <v>123</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F9" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9500efa0c7e64d2d31ad4801672dc910</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>e023b8fc433d610812ecfb71337b588d</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
           <t>C</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>123</v>
+      <c r="C10" t="n">
+        <v>123</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F10" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>b6467f9b8b7b84ac4fc8c475fb490e61</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>f955dcdea3583274bcb68245c30be141</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>123</v>
+      <c r="C11" t="n">
+        <v>123</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F11" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>72058c0774700d07ccbcc37f694d38b9</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>f2215d9ecc12fc0472668f00274e943d</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>123</v>
+      <c r="C12" t="n">
+        <v>123</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F12" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>7e14d84bfb5e59bb90eb616e2ec54ace</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1d0b15c60c59ae39d4159f7bc42fadb2</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
           <t>C</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>123</v>
+      <c r="C13" t="n">
+        <v>123</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F13" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>4828cfa312ccc419df606e3044aaeac9</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>bd5341391d581ca633c79cc21b35aca2</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>123</v>
+      <c r="C14" t="n">
+        <v>123</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F14" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>9d29393718b21e1edbf28eabcf8ab52a</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>960d298c1e4e805b67153ef9aff17811</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="D15" t="n">
-        <v>123</v>
+      <c r="C15" t="n">
+        <v>123</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F15" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>a341c527599003ffa1446e19c60e0f0f</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>46184e5bd19db955c510fd512e9a942d</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
           <t>C</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>123</v>
+      <c r="C16" t="n">
+        <v>123</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F16" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1b7aa943a07f27297cbd2ff78d378156</t>
+        </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>5fdd9a6b43990bd19d8eb52bd9fc0942</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="D17" t="n">
-        <v>123</v>
+      <c r="C17" t="n">
+        <v>123</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F17" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>5f1a5a83cdbe0dc39f5b5742f13a6a2e</t>
+        </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1ae6228366781905bc427bbc1306dd37</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="D18" t="n">
-        <v>123</v>
+      <c r="C18" t="n">
+        <v>123</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F18" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>98b426fc509bbba2015759bcb93333bf</t>
+        </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3b31c3488ffe1b5ae3f5378476bf9391</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
           <t>C</t>
         </is>
       </c>
-      <c r="D19" t="n">
-        <v>123</v>
+      <c r="C19" t="n">
+        <v>123</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F19" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2758f80410d156e934dfe6ebf64668b1</t>
+        </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4ad877f9ad921e35e3727467323092bc</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>123</v>
+      <c r="C20" t="n">
+        <v>123</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F20" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ad627c1a38aacd2df6a7c598611e6e3e</t>
+        </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>354de01989a7e2732b9e9834fbab22a5</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="D21" t="n">
-        <v>123</v>
+      <c r="C21" t="n">
+        <v>123</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F21" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>5b3023428acd66bbaefdc52df4a1c7b7</t>
+        </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>a13d67e2fc8f3dad5dffc8ae113008ea</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
           <t>C</t>
         </is>
       </c>
-      <c r="D22" t="n">
-        <v>123</v>
+      <c r="C22" t="n">
+        <v>123</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
-      <c r="F22" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>cb91573fd48aa30a9de080c2c997e5c1</t>
+        </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1ec7db1e158eb989802c57539b4fb2a3</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="D23" t="n">
-        <v>123</v>
+      <c r="C23" t="n">
+        <v>123</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>44056.42328599537</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>44056.42328599537</v>
-      </c>
-      <c r="F23" s="2" t="n">
         <v>44056.42328599537</v>
       </c>
     </row>

</xml_diff>